<commit_message>
Push an update for VSL occupation
</commit_message>
<xml_diff>
--- a/VSL_Occupation/VSL Data for ChatGPT v2.xlsx
+++ b/VSL_Occupation/VSL Data for ChatGPT v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23081e3b81f5d0e4/Desktop/AI_Programming/VSL_Occupation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{784C1221-E738-4588-A2E5-E490E3E8E0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8AAE2F2-CA39-4026-9D5C-00DD44032815}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{784C1221-E738-4588-A2E5-E490E3E8E0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6391DC3C-9F38-4120-BD47-18E40C543429}"/>
   <bookViews>
     <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="153">
   <si>
     <t>ANSZIC Code</t>
   </si>
@@ -751,6 +751,16 @@
   </si>
   <si>
     <t>Building and Other Industrial Cleaning Services</t>
+  </si>
+  <si>
+    <t>Class Action Description</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>* DST Legal has filed a class action lawsuit against GrainCorp. The class action is on behalf of residents living near the GrainCorp oilseed factor in rural Victoria. The class action alleges that the defendant allegedly operated a plant that continuously emitted excessively loud noise and offensive odour, constituting tortious nuisance and breaching the Environmental Protection Act. Case in progress
+* Maurice Blackburn has settled a class action lawsuit against Thanh Phu. The class action was on behalf of people who consumed contaminated food. Thanh Phu Pty Ltd sold salmonella contaminated food from its store leading to many people being hospitalised and one man died Settled for unknown amount</t>
   </si>
 </sst>
 </file>
@@ -816,6 +826,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1084,10 +1098,10 @@
   <sheetPr codeName="Sheet24">
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,10 +1109,11 @@
     <col min="1" max="1" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="88.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="6" max="6" width="255.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1114,8 +1129,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -1131,8 +1149,11 @@
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="F2" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
@@ -1148,8 +1169,11 @@
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
@@ -1165,8 +1189,11 @@
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F4" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
@@ -1182,8 +1209,11 @@
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>100</v>
       </c>
@@ -1199,8 +1229,11 @@
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>102</v>
       </c>
@@ -1216,8 +1249,11 @@
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F7" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>104</v>
       </c>
@@ -1233,8 +1269,11 @@
       <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>106</v>
       </c>
@@ -1250,8 +1289,11 @@
       <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F9" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>108</v>
       </c>
@@ -1267,8 +1309,11 @@
       <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F10" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>110</v>
       </c>
@@ -1284,8 +1329,11 @@
       <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="F11" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>112</v>
       </c>
@@ -1301,8 +1349,11 @@
       <c r="E12" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F12" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>114</v>
       </c>
@@ -1318,8 +1369,11 @@
       <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F13" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>116</v>
       </c>
@@ -1335,8 +1389,11 @@
       <c r="E14" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="F14" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
@@ -1352,8 +1409,11 @@
       <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F15" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>120</v>
       </c>
@@ -1369,8 +1429,11 @@
       <c r="E16" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F16" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>122</v>
       </c>
@@ -1386,8 +1449,11 @@
       <c r="E17" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F17" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>124</v>
       </c>
@@ -1403,8 +1469,11 @@
       <c r="E18" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F18" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>126</v>
       </c>
@@ -1420,8 +1489,11 @@
       <c r="E19" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F19" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>128</v>
       </c>
@@ -1437,8 +1509,11 @@
       <c r="E20" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F20" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>130</v>
       </c>
@@ -1454,8 +1529,11 @@
       <c r="E21" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>132</v>
       </c>
@@ -1471,8 +1549,11 @@
       <c r="E22" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F22" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>134</v>
       </c>
@@ -1488,8 +1569,11 @@
       <c r="E23" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F23" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>136</v>
       </c>
@@ -1505,8 +1589,11 @@
       <c r="E24" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F24" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>138</v>
       </c>
@@ -1522,8 +1609,11 @@
       <c r="E25" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="F25" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>140</v>
       </c>
@@ -1539,8 +1629,11 @@
       <c r="E26" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="F26" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>142</v>
       </c>
@@ -1556,8 +1649,11 @@
       <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="F27" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>144</v>
       </c>
@@ -1573,8 +1669,11 @@
       <c r="E28" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F28" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>146</v>
       </c>
@@ -1590,8 +1689,11 @@
       <c r="E29" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="F29" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>148</v>
       </c>
@@ -1606,6 +1708,9 @@
       </c>
       <c r="E30" s="2" t="s">
         <v>91</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>